<commit_message>
Added questions for today
</commit_message>
<xml_diff>
--- a/revise.xlsx
+++ b/revise.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shivanssingh82/Desktop/Practice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ParikshitJ/Desktop/Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>http:www.spoj.comproblemsRAINBOW</t>
   </si>
@@ -120,6 +120,30 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>a-data-structure-question</t>
+  </si>
+  <si>
+    <t>find-first-non-repeating-character-stream-characters</t>
+  </si>
+  <si>
+    <t>check-divisibility-binary-stream</t>
+  </si>
+  <si>
+    <t>select-a-random-number-from-stream-with-o1-space</t>
+  </si>
+  <si>
+    <t>connect-n-ropes-minimum-cost</t>
+  </si>
+  <si>
+    <t>minimum-sum-squares-characters-counts-given-string-removing-k-characters</t>
+  </si>
+  <si>
+    <t>median-of-stream-of-integers-running-integers</t>
+  </si>
+  <si>
+    <t>lru-cache-implementation</t>
   </si>
 </sst>
 </file>
@@ -454,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,6 +667,46 @@
         <v>24</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:B29">
     <sortCondition ref="A1"/>

</xml_diff>